<commit_message>
esboço da página de vinculação de aluno/paciente feita
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema próprio odonto\julho-2023 POC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema_odonto\proof_of_concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640CB357-A576-46DF-AB77-C6E90C772F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FED1C3-FC62-4D10-ABB3-85CB0C498EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Paciente</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>Produção por responsável técnico</t>
+  </si>
+  <si>
+    <t>vinculo-pacientes</t>
+  </si>
+  <si>
+    <t>pacientes-disciplina</t>
+  </si>
+  <si>
+    <t>ano/semestre</t>
   </si>
 </sst>
 </file>
@@ -433,7 +442,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -759,7 +768,7 @@
   <dimension ref="B2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +914,9 @@
       <c r="F7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="H7" s="3" t="s">
         <v>80</v>
       </c>
@@ -926,7 +937,9 @@
       <c r="F8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="H8" s="3" t="s">
         <v>81</v>
       </c>
@@ -1014,7 +1027,9 @@
       <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">

</xml_diff>

<commit_message>
esboço de bind function na página de vinculação
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema_odonto\proof_of_concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FED1C3-FC62-4D10-ABB3-85CB0C498EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98E795E-FB8E-40C1-9D1E-F8571D813491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Paciente</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>ano/semestre</t>
+  </si>
+  <si>
+    <t>DEMANDA-COMPLEXIDADE</t>
   </si>
 </sst>
 </file>
@@ -765,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5035DA7-7C4F-4E71-8F51-262E3B1D2C20}">
-  <dimension ref="B2:H33"/>
+  <dimension ref="B2:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,46 +1076,51 @@
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new version for perfil w/ tabs
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema_odonto\proof_of_concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98E795E-FB8E-40C1-9D1E-F8571D813491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBEAAEE-D9D0-4F05-89D1-8A353293A8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Variáveis" sheetId="1" r:id="rId1"/>
+    <sheet name="Options" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
   <si>
     <t>Paciente</t>
   </si>
@@ -48,9 +49,6 @@
     <t>NOME</t>
   </si>
   <si>
-    <t>CNS</t>
-  </si>
-  <si>
     <t>RG</t>
   </si>
   <si>
@@ -286,13 +284,73 @@
   </si>
   <si>
     <t>DEMANDA-COMPLEXIDADE</t>
+  </si>
+  <si>
+    <t>Status paciente</t>
+  </si>
+  <si>
+    <t>Em espera</t>
+  </si>
+  <si>
+    <t>Em atendimento</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Abandono/Desistência</t>
+  </si>
+  <si>
+    <t>Continua em tratamento na disciplina/especialidade</t>
+  </si>
+  <si>
+    <t>Nível de complexidade</t>
+  </si>
+  <si>
+    <t>Escolher</t>
+  </si>
+  <si>
+    <t>1 - Baixa</t>
+  </si>
+  <si>
+    <t>2 - Média</t>
+  </si>
+  <si>
+    <t>3 - Alta (Pós-graduação)</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>VARIÁVEIS</t>
+  </si>
+  <si>
+    <t>FAZER</t>
+  </si>
+  <si>
+    <t>ADD CNS NO PERFIL DO PACIENTE</t>
+  </si>
+  <si>
+    <t>ADD UM "ODONTOGRAMA" NO PERFIL DO PACIENTE</t>
+  </si>
+  <si>
+    <t>JS para vinculação</t>
+  </si>
+  <si>
+    <t>Separa páginas de vinculação e desvinculação?</t>
+  </si>
+  <si>
+    <t>Cartão SUS (CNS)</t>
+  </si>
+  <si>
+    <t>já add no "perfil com TABS"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,8 +366,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,8 +394,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -420,11 +492,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -454,6 +579,64 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5035DA7-7C4F-4E71-8F51-262E3B1D2C20}">
-  <dimension ref="B2:H34"/>
+  <dimension ref="B2:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,349 +966,534 @@
     <col min="5" max="5" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="11" max="11" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
+      <c r="J2" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2" s="29"/>
+      <c r="L2" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="19"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="20"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="28"/>
+    </row>
+    <row r="4" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="24">
+        <v>1</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="25">
+        <v>2</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="25">
+        <v>3</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="L6" s="30"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="25">
+        <v>4</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="30"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="25">
+        <v>5</v>
+      </c>
+      <c r="K8" s="26"/>
+      <c r="L8" s="30"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" s="25">
+        <v>6</v>
+      </c>
+      <c r="K9" s="26"/>
+      <c r="L9" s="30"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="G10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="25">
+        <v>7</v>
+      </c>
+      <c r="K10" s="26"/>
+      <c r="L10" s="30"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="25">
+        <v>8</v>
+      </c>
+      <c r="K11" s="26"/>
+      <c r="L11" s="30"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="J12" s="25">
+        <v>9</v>
+      </c>
+      <c r="K12" s="26"/>
+      <c r="L12" s="30"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="J13" s="25">
+        <v>10</v>
+      </c>
+      <c r="K13" s="26"/>
+      <c r="L13" s="30"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="19"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="20"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="C40" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="14"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B38:H39"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="J2:K3"/>
+    <mergeCell ref="L2:L3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBC8570-734E-4686-8E79-8469335D18A4}">
+  <dimension ref="B1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="14" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
desmembramento de vincular e desvincular paciente
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema_odonto\proof_of_concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FD0385-1D95-4450-A18B-4F0EEC28B48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB326C-B5C0-48A6-B42B-3483B86A68CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t>Paciente</t>
   </si>
@@ -100,126 +100,24 @@
     <t>CIDADE</t>
   </si>
   <si>
-    <t>DEMANDA-ÁREA DA SAÚDE</t>
-  </si>
-  <si>
-    <t>DEMANDA-ESPECIALIDADE</t>
-  </si>
-  <si>
-    <t>DEMANDA-ESPECÍFICA</t>
-  </si>
-  <si>
-    <t>DATA DO ENCAMINHAMENTO</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
-    <t>DATA-PROCEDIMENTO</t>
-  </si>
-  <si>
-    <t>PROCEDIMENTO</t>
-  </si>
-  <si>
-    <t>ALUNO-PROCEDIMENTO</t>
-  </si>
-  <si>
-    <t>RESPONSÁVEL-PROCEDIMENTO</t>
-  </si>
-  <si>
-    <t>FILE-EXAME COMPLEMENTAR</t>
-  </si>
-  <si>
-    <t>TIPO-EXAME COMPLEMENTAR</t>
-  </si>
-  <si>
-    <t>DESCRIÇÃO-EXAME COMPLEMENTAR</t>
-  </si>
-  <si>
-    <t>DATA-EXAME COMPLEMENTAR</t>
-  </si>
-  <si>
     <t>código</t>
   </si>
   <si>
-    <t>componente curricular</t>
-  </si>
-  <si>
-    <t>público-alvo geral</t>
-  </si>
-  <si>
-    <t>tipos de casos</t>
-  </si>
-  <si>
     <t>Relatórios</t>
   </si>
   <si>
     <t>lista por status</t>
   </si>
   <si>
-    <t>bloco de pacientes</t>
-  </si>
-  <si>
-    <t>agenda de clínicas</t>
-  </si>
-  <si>
-    <t>status-agendamento</t>
-  </si>
-  <si>
-    <t>data-agendamento</t>
-  </si>
-  <si>
     <t>vínculo-PacAluno</t>
   </si>
   <si>
     <t>justificativa-vinculação</t>
   </si>
   <si>
-    <t>homologar-vinculação</t>
-  </si>
-  <si>
-    <t>lista de códigos</t>
-  </si>
-  <si>
-    <t>produção_SUS</t>
-  </si>
-  <si>
-    <t>lista de materiais</t>
-  </si>
-  <si>
-    <t>qtd_materiais</t>
-  </si>
-  <si>
-    <t>tipo_material</t>
-  </si>
-  <si>
-    <t>encaminhar-paciente</t>
-  </si>
-  <si>
-    <t>aprovar-encaminhamento</t>
-  </si>
-  <si>
-    <t>homologar-encaminhamento</t>
-  </si>
-  <si>
-    <t>encaminhamento-data</t>
-  </si>
-  <si>
-    <t>encaminhamento-justificativa</t>
-  </si>
-  <si>
-    <t>encaminhamento-DE</t>
-  </si>
-  <si>
-    <t>encaminhamento-PARA</t>
-  </si>
-  <si>
-    <t>encaminhamento-demanda</t>
-  </si>
-  <si>
-    <t>encaminhamento-professor</t>
-  </si>
-  <si>
     <t>Relatório de altas por disciplina, turma ou semestre</t>
   </si>
   <si>
@@ -232,39 +130,6 @@
     <t>Administração</t>
   </si>
   <si>
-    <t>lotar-responsável</t>
-  </si>
-  <si>
-    <t>atendimento-data</t>
-  </si>
-  <si>
-    <t>atendimento-codSUS</t>
-  </si>
-  <si>
-    <t>atendimento-descrição</t>
-  </si>
-  <si>
-    <t>atendimento-responsável</t>
-  </si>
-  <si>
-    <t>prontuários-específicos</t>
-  </si>
-  <si>
-    <t>avaliar-pontualidade</t>
-  </si>
-  <si>
-    <t>avaliar-conhecimento</t>
-  </si>
-  <si>
-    <t>avaliar-postura</t>
-  </si>
-  <si>
-    <t>avaliar-desempenho</t>
-  </si>
-  <si>
-    <t>média atendimentos</t>
-  </si>
-  <si>
     <t>Produção por estudante</t>
   </si>
   <si>
@@ -274,18 +139,6 @@
     <t>Produção por responsável técnico</t>
   </si>
   <si>
-    <t>vinculo-pacientes</t>
-  </si>
-  <si>
-    <t>pacientes-disciplina</t>
-  </si>
-  <si>
-    <t>ano/semestre</t>
-  </si>
-  <si>
-    <t>DEMANDA-COMPLEXIDADE</t>
-  </si>
-  <si>
     <t>Status paciente</t>
   </si>
   <si>
@@ -344,6 +197,159 @@
   </si>
   <si>
     <t>falta incluir no backend</t>
+  </si>
+  <si>
+    <t>pacientesAtendidos</t>
+  </si>
+  <si>
+    <t>vinculoPacientes</t>
+  </si>
+  <si>
+    <t>mediaAtendimentos</t>
+  </si>
+  <si>
+    <t>atendimentoResponsável</t>
+  </si>
+  <si>
+    <t>atendimentoDescrição</t>
+  </si>
+  <si>
+    <t>atendimentoCodSUS</t>
+  </si>
+  <si>
+    <t>atendimentoData</t>
+  </si>
+  <si>
+    <t>encaminhamentoProfessor</t>
+  </si>
+  <si>
+    <t>encaminhamentoJustificativa</t>
+  </si>
+  <si>
+    <t>encaminhamentoDemanda</t>
+  </si>
+  <si>
+    <t>encaminhamentoPara</t>
+  </si>
+  <si>
+    <t>encaminhamentoDe</t>
+  </si>
+  <si>
+    <t>encaminhamentoData</t>
+  </si>
+  <si>
+    <t>encaminharPaciente</t>
+  </si>
+  <si>
+    <t>alunoProcedimento</t>
+  </si>
+  <si>
+    <t>responsavelProcedimento</t>
+  </si>
+  <si>
+    <t>aprovarEncaminhamento</t>
+  </si>
+  <si>
+    <t>avaliarPontualidade</t>
+  </si>
+  <si>
+    <t>avaliarConhecimento</t>
+  </si>
+  <si>
+    <t>avaliarPostura</t>
+  </si>
+  <si>
+    <t>avaliarDesempenho</t>
+  </si>
+  <si>
+    <t>homologarEncaminhamento</t>
+  </si>
+  <si>
+    <t>homologarVinculação</t>
+  </si>
+  <si>
+    <t>dataAgendamento</t>
+  </si>
+  <si>
+    <t>statusAgendamento</t>
+  </si>
+  <si>
+    <t>agendaClínicas</t>
+  </si>
+  <si>
+    <t>listaCodSUS</t>
+  </si>
+  <si>
+    <t>producaoSUS</t>
+  </si>
+  <si>
+    <t>listaMateriais</t>
+  </si>
+  <si>
+    <t>qtdMateriais</t>
+  </si>
+  <si>
+    <t>tipoMateriais</t>
+  </si>
+  <si>
+    <t>lotarResponsavel</t>
+  </si>
+  <si>
+    <t>prontuarioEspecifico</t>
+  </si>
+  <si>
+    <t>componenteCurricular</t>
+  </si>
+  <si>
+    <t>publicoAlvo</t>
+  </si>
+  <si>
+    <t>tipoCasos</t>
+  </si>
+  <si>
+    <t>pacientesDisciplina</t>
+  </si>
+  <si>
+    <t>anoSemestre</t>
+  </si>
+  <si>
+    <t>demandaAreaSaude</t>
+  </si>
+  <si>
+    <t>demandaEspecialidade</t>
+  </si>
+  <si>
+    <t>demandaComplexidade</t>
+  </si>
+  <si>
+    <t>demandaEspecifica</t>
+  </si>
+  <si>
+    <t>demandaData</t>
+  </si>
+  <si>
+    <t>statusPaciente</t>
+  </si>
+  <si>
+    <t>prioridade (boolean)</t>
+  </si>
+  <si>
+    <t>procedimentoData</t>
+  </si>
+  <si>
+    <t>procedimentoDescricao</t>
+  </si>
+  <si>
+    <t>exameData</t>
+  </si>
+  <si>
+    <t>exameDescricao</t>
+  </si>
+  <si>
+    <t>exameTipo</t>
+  </si>
+  <si>
+    <t>exameFile</t>
   </si>
 </sst>
 </file>
@@ -555,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,9 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -607,30 +610,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -642,6 +621,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -958,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5035DA7-7C4F-4E71-8F51-262E3B1D2C20}">
-  <dimension ref="B2:L45"/>
+  <dimension ref="B2:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,273 +989,271 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="J2" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="26" t="s">
-        <v>28</v>
+      <c r="B2" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="J2" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="29"/>
+      <c r="L2" s="30" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="30"/>
     </row>
     <row r="4" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="F4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="27">
+      <c r="H4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="18">
         <v>1</v>
       </c>
-      <c r="K4" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>105</v>
+      <c r="K4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>31</v>
+      <c r="C5" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="30">
+        <v>27</v>
+      </c>
+      <c r="J5" s="21">
         <v>2</v>
       </c>
-      <c r="K5" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="L5" s="29" t="s">
-        <v>105</v>
+      <c r="K5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="16">
+        <v>3</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" s="17">
-        <v>3</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="L6" s="18"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
+      <c r="C7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="17">
+        <v>31</v>
+      </c>
+      <c r="J7" s="16">
         <v>4</v>
       </c>
-      <c r="K7" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="L7" s="18"/>
+      <c r="K7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="17"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>60</v>
+      <c r="C8" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="17">
+        <v>32</v>
+      </c>
+      <c r="J8" s="16">
         <v>5</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="18"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="17"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>61</v>
+      <c r="C9" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9" s="17">
+        <v>34</v>
+      </c>
+      <c r="J9" s="16">
         <v>6</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="18"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="17"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>62</v>
+      <c r="C10" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>75</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="17">
+        <v>35</v>
+      </c>
+      <c r="J10" s="16">
         <v>7</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="18"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="17"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>59</v>
+      <c r="C11" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J11" s="17">
+        <v>36</v>
+      </c>
+      <c r="J11" s="16">
         <v>8</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="18"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="17"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>63</v>
+      <c r="C12" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>77</v>
@@ -1255,74 +1262,77 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="J12" s="17">
+      <c r="J12" s="16">
         <v>9</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="18"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="17"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>69</v>
+      <c r="C13" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="J13" s="17">
+      <c r="J13" s="16">
         <v>10</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="18"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="17"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>70</v>
+      <c r="C14" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>71</v>
+      <c r="C15" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>72</v>
+      <c r="C16" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>78</v>
+      <c r="C17" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>82</v>
+      <c r="C18" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="C19" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
@@ -1351,133 +1361,138 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="21"/>
+      <c r="B36" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="22"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="24"/>
+      <c r="B39" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="25"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>92</v>
-      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="28"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>93</v>
+      <c r="B41" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>96</v>
+      <c r="B42" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="14"/>
+      <c r="B45" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B38:H39"/>
+    <mergeCell ref="B39:H40"/>
     <mergeCell ref="B2:H3"/>
     <mergeCell ref="J2:K3"/>
     <mergeCell ref="L2:L3"/>
@@ -1497,8 +1512,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="13" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add página cadastrar material com script para inclusão na tabela
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema_odonto\proof_of_concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB326C-B5C0-48A6-B42B-3483B86A68CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0C7753-91A5-40B3-8738-F42D052BC7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
   <si>
     <t>Paciente</t>
   </si>
@@ -190,9 +190,6 @@
     <t>JS para vinculação</t>
   </si>
   <si>
-    <t>Separa páginas de vinculação e desvinculação?</t>
-  </si>
-  <si>
     <t>Cartão SUS (CNS)</t>
   </si>
   <si>
@@ -283,15 +280,6 @@
     <t>producaoSUS</t>
   </si>
   <si>
-    <t>listaMateriais</t>
-  </si>
-  <si>
-    <t>qtdMateriais</t>
-  </si>
-  <si>
-    <t>tipoMateriais</t>
-  </si>
-  <si>
     <t>lotarResponsavel</t>
   </si>
   <si>
@@ -350,6 +338,42 @@
   </si>
   <si>
     <t>exameFile</t>
+  </si>
+  <si>
+    <t>Desmembramento de página vincular e desvincular</t>
+  </si>
+  <si>
+    <t>ok!</t>
+  </si>
+  <si>
+    <t>qtdMaterial</t>
+  </si>
+  <si>
+    <t>tipoMaterial</t>
+  </si>
+  <si>
+    <t>codMaterial</t>
+  </si>
+  <si>
+    <t>nomeMaterial</t>
+  </si>
+  <si>
+    <t>Lista de materiais</t>
+  </si>
+  <si>
+    <t>Lista Códigos Sus</t>
+  </si>
+  <si>
+    <t>listaMaterial</t>
+  </si>
+  <si>
+    <t>codSUS</t>
+  </si>
+  <si>
+    <t>procedimentoSUS</t>
+  </si>
+  <si>
+    <t>qtdSUS (ano/semestre)</t>
   </si>
 </sst>
 </file>
@@ -623,6 +647,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -646,12 +676,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -969,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5035DA7-7C4F-4E71-8F51-262E3B1D2C20}">
   <dimension ref="B2:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,34 +1013,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="J2" s="29" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="J2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="30"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="32"/>
     </row>
     <row r="4" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1047,7 +1071,7 @@
         <v>51</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -1055,14 +1079,14 @@
         <v>5</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>25</v>
@@ -1077,7 +1101,7 @@
         <v>52</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -1085,19 +1109,19 @@
         <v>6</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>30</v>
@@ -1106,28 +1130,30 @@
         <v>3</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="L6" s="17"/>
+        <v>104</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>31</v>
@@ -1136,7 +1162,7 @@
         <v>4</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L7" s="17"/>
     </row>
@@ -1145,19 +1171,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>32</v>
@@ -1173,19 +1199,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>34</v>
@@ -1201,19 +1227,17 @@
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>88</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>35</v>
@@ -1229,15 +1253,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
         <v>36</v>
@@ -1253,10 +1275,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1273,7 +1295,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1291,7 +1313,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -1299,7 +1321,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -1307,142 +1329,169 @@
         <v>15</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F21" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="27"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="26"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="28"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="30"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">

</xml_diff>

<commit_message>
front-end com scripts para vincular-2.html e desvincular-2.html
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema-odonto\proof-of-concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03634842-F06F-4C28-AF7D-ECDB520F1D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB5266F-9C0A-46AC-9C6A-F4D4295E5575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Variáveis" sheetId="1" r:id="rId1"/>
@@ -43,63 +43,6 @@
     <t>Disciplinas</t>
   </si>
   <si>
-    <t>CPF</t>
-  </si>
-  <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>RG</t>
-  </si>
-  <si>
-    <t>DATA DE NASCIMENTO</t>
-  </si>
-  <si>
-    <t>E-MAIL</t>
-  </si>
-  <si>
-    <t>TELEFONE</t>
-  </si>
-  <si>
-    <t>ESTADO CIVIL</t>
-  </si>
-  <si>
-    <t>SEXO</t>
-  </si>
-  <si>
-    <t>COR/RAÇA</t>
-  </si>
-  <si>
-    <t>NOME DO PAI</t>
-  </si>
-  <si>
-    <t>NOME DA MÃE</t>
-  </si>
-  <si>
-    <t>PNE</t>
-  </si>
-  <si>
-    <t>TIPO DE ENDEREÇO</t>
-  </si>
-  <si>
-    <t>CEP</t>
-  </si>
-  <si>
-    <t>ENDEREÇO</t>
-  </si>
-  <si>
-    <t>NÚMERO</t>
-  </si>
-  <si>
-    <t>COMPLEMENTO</t>
-  </si>
-  <si>
-    <t>BAIRRO</t>
-  </si>
-  <si>
-    <t>CIDADE</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -142,21 +85,6 @@
     <t>Status paciente</t>
   </si>
   <si>
-    <t>Em espera</t>
-  </si>
-  <si>
-    <t>Em atendimento</t>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Abandono/Desistência</t>
-  </si>
-  <si>
-    <t>Continua em tratamento na disciplina/especialidade</t>
-  </si>
-  <si>
     <t>Nível de complexidade</t>
   </si>
   <si>
@@ -187,9 +115,6 @@
     <t>ADD UM "ODONTOGRAMA" NO PERFIL DO PACIENTE</t>
   </si>
   <si>
-    <t>Cartão SUS (CNS)</t>
-  </si>
-  <si>
     <t>falta incluir no backend</t>
   </si>
   <si>
@@ -380,6 +305,81 @@
   </si>
   <si>
     <t>justificativaSolicitacao</t>
+  </si>
+  <si>
+    <t>pacienteCPF</t>
+  </si>
+  <si>
+    <t>pacienteNome</t>
+  </si>
+  <si>
+    <t>pacienteSUS</t>
+  </si>
+  <si>
+    <t>pacienteRG</t>
+  </si>
+  <si>
+    <t>pacienteNasc</t>
+  </si>
+  <si>
+    <t>pacienteEmail</t>
+  </si>
+  <si>
+    <t>pacienteFone</t>
+  </si>
+  <si>
+    <t>pacienteEstCivil</t>
+  </si>
+  <si>
+    <t>pacienteSexo</t>
+  </si>
+  <si>
+    <t>pacienteCor</t>
+  </si>
+  <si>
+    <t>pacienteMae</t>
+  </si>
+  <si>
+    <t>pacientePai</t>
+  </si>
+  <si>
+    <t>pacientePNE</t>
+  </si>
+  <si>
+    <t>pacienteEndereço</t>
+  </si>
+  <si>
+    <t>pacienteCEP</t>
+  </si>
+  <si>
+    <t>pacienteTipoEndereço</t>
+  </si>
+  <si>
+    <t>pacienteEndNum</t>
+  </si>
+  <si>
+    <t>pacienteEndComp</t>
+  </si>
+  <si>
+    <t>pacienteBairro</t>
+  </si>
+  <si>
+    <t>pacienteCidade</t>
+  </si>
+  <si>
+    <t>continuaTratamento</t>
+  </si>
+  <si>
+    <t>emAtendimento</t>
+  </si>
+  <si>
+    <t>emEspera</t>
+  </si>
+  <si>
+    <t>altaPaciente</t>
+  </si>
+  <si>
+    <t>abandonoPaciente</t>
   </si>
 </sst>
 </file>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5035DA7-7C4F-4E71-8F51-262E3B1D2C20}">
   <dimension ref="B2:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1020,7 @@
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -1029,11 +1029,11 @@
       <c r="G2" s="26"/>
       <c r="H2" s="27"/>
       <c r="J2" s="31" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="K2" s="31"/>
       <c r="L2" s="32" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1062,133 +1062,133 @@
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="J4" s="18">
         <v>1</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="J5" s="21">
         <v>2</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="J6" s="16">
         <v>3</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="L6" s="16"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="J7" s="16">
         <v>4</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="L7" s="17"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="J8" s="16">
         <v>5</v>
@@ -1198,23 +1198,23 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="J9" s="16">
         <v>6</v>
@@ -1224,21 +1224,21 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="J10" s="16">
         <v>7</v>
@@ -1248,19 +1248,19 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="J11" s="16">
         <v>8</v>
@@ -1270,13 +1270,13 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1290,10 +1290,10 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1308,190 +1308,190 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="25" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
@@ -1511,47 +1511,47 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="12" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="C46" s="13"/>
     </row>

</xml_diff>

<commit_message>
novas htmls em desenvolvimento
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema-odonto\proof-of-concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB5266F-9C0A-46AC-9C6A-F4D4295E5575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C37E33-28D0-439B-9A54-E09D5440CFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Variáveis" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="277">
   <si>
     <t>Paciente</t>
   </si>
@@ -229,9 +229,6 @@
     <t>exameData</t>
   </si>
   <si>
-    <t>exameDescricao</t>
-  </si>
-  <si>
     <t>exameTipo</t>
   </si>
   <si>
@@ -380,13 +377,493 @@
   </si>
   <si>
     <t>abandonoPaciente</t>
+  </si>
+  <si>
+    <t>página de registrar demanda / deletar uma tabela, corrigir SCRIPT APARECENDO</t>
+  </si>
+  <si>
+    <t>odontograma11</t>
+  </si>
+  <si>
+    <t>odontograma12</t>
+  </si>
+  <si>
+    <t>odontograma13</t>
+  </si>
+  <si>
+    <t>odontograma14</t>
+  </si>
+  <si>
+    <t>odontograma15</t>
+  </si>
+  <si>
+    <t>odontograma16</t>
+  </si>
+  <si>
+    <t>odontograma17</t>
+  </si>
+  <si>
+    <t>odontograma18</t>
+  </si>
+  <si>
+    <t>odontograma21</t>
+  </si>
+  <si>
+    <t>odontograma22</t>
+  </si>
+  <si>
+    <t>odontograma23</t>
+  </si>
+  <si>
+    <t>odontograma24</t>
+  </si>
+  <si>
+    <t>odontograma25</t>
+  </si>
+  <si>
+    <t>odontograma26</t>
+  </si>
+  <si>
+    <t>odontograma27</t>
+  </si>
+  <si>
+    <t>odontograma28</t>
+  </si>
+  <si>
+    <t>odontograma31</t>
+  </si>
+  <si>
+    <t>odontograma32</t>
+  </si>
+  <si>
+    <t>odontograma33</t>
+  </si>
+  <si>
+    <t>odontograma34</t>
+  </si>
+  <si>
+    <t>odontograma35</t>
+  </si>
+  <si>
+    <t>odontograma36</t>
+  </si>
+  <si>
+    <t>odontograma37</t>
+  </si>
+  <si>
+    <t>odontograma38</t>
+  </si>
+  <si>
+    <t>odontograma41</t>
+  </si>
+  <si>
+    <t>odontograma42</t>
+  </si>
+  <si>
+    <t>odontograma43</t>
+  </si>
+  <si>
+    <t>odontograma44</t>
+  </si>
+  <si>
+    <t>odontograma45</t>
+  </si>
+  <si>
+    <t>odontograma46</t>
+  </si>
+  <si>
+    <t>odontograma47</t>
+  </si>
+  <si>
+    <t>odontograma48</t>
+  </si>
+  <si>
+    <t>odontograma51</t>
+  </si>
+  <si>
+    <t>odontograma52</t>
+  </si>
+  <si>
+    <t>odontograma53</t>
+  </si>
+  <si>
+    <t>odontograma54</t>
+  </si>
+  <si>
+    <t>odontograma55</t>
+  </si>
+  <si>
+    <t>odontograma61</t>
+  </si>
+  <si>
+    <t>odontograma62</t>
+  </si>
+  <si>
+    <t>odontograma63</t>
+  </si>
+  <si>
+    <t>odontograma64</t>
+  </si>
+  <si>
+    <t>odontograma65</t>
+  </si>
+  <si>
+    <t>odontograma71</t>
+  </si>
+  <si>
+    <t>odontograma72</t>
+  </si>
+  <si>
+    <t>odontograma73</t>
+  </si>
+  <si>
+    <t>odontograma74</t>
+  </si>
+  <si>
+    <t>odontograma75</t>
+  </si>
+  <si>
+    <t>odontograma81</t>
+  </si>
+  <si>
+    <t>odontograma82</t>
+  </si>
+  <si>
+    <t>odontograma83</t>
+  </si>
+  <si>
+    <t>odontograma84</t>
+  </si>
+  <si>
+    <t>odontograma85</t>
+  </si>
+  <si>
+    <t>ipv11</t>
+  </si>
+  <si>
+    <t>ipv12</t>
+  </si>
+  <si>
+    <t>ipv13</t>
+  </si>
+  <si>
+    <t>ipv14</t>
+  </si>
+  <si>
+    <t>ipv15</t>
+  </si>
+  <si>
+    <t>ipv16</t>
+  </si>
+  <si>
+    <t>ipv17</t>
+  </si>
+  <si>
+    <t>ipv18</t>
+  </si>
+  <si>
+    <t>ipv21</t>
+  </si>
+  <si>
+    <t>ipv22</t>
+  </si>
+  <si>
+    <t>ipv23</t>
+  </si>
+  <si>
+    <t>ipv24</t>
+  </si>
+  <si>
+    <t>ipv25</t>
+  </si>
+  <si>
+    <t>ipv26</t>
+  </si>
+  <si>
+    <t>ipv27</t>
+  </si>
+  <si>
+    <t>ipv28</t>
+  </si>
+  <si>
+    <t>ipv31</t>
+  </si>
+  <si>
+    <t>ipv32</t>
+  </si>
+  <si>
+    <t>ipv33</t>
+  </si>
+  <si>
+    <t>ipv34</t>
+  </si>
+  <si>
+    <t>ipv35</t>
+  </si>
+  <si>
+    <t>ipv36</t>
+  </si>
+  <si>
+    <t>ipv37</t>
+  </si>
+  <si>
+    <t>ipv38</t>
+  </si>
+  <si>
+    <t>ipv41</t>
+  </si>
+  <si>
+    <t>ipv42</t>
+  </si>
+  <si>
+    <t>ipv43</t>
+  </si>
+  <si>
+    <t>ipv44</t>
+  </si>
+  <si>
+    <t>ipv45</t>
+  </si>
+  <si>
+    <t>isg11</t>
+  </si>
+  <si>
+    <t>prof11</t>
+  </si>
+  <si>
+    <t>prof12</t>
+  </si>
+  <si>
+    <t>prof13</t>
+  </si>
+  <si>
+    <t>prof14</t>
+  </si>
+  <si>
+    <t>prof15</t>
+  </si>
+  <si>
+    <t>prof16</t>
+  </si>
+  <si>
+    <t>prof17</t>
+  </si>
+  <si>
+    <t>prof18</t>
+  </si>
+  <si>
+    <t>prof21</t>
+  </si>
+  <si>
+    <t>prof22</t>
+  </si>
+  <si>
+    <t>prof23</t>
+  </si>
+  <si>
+    <t>prof24</t>
+  </si>
+  <si>
+    <t>prof25</t>
+  </si>
+  <si>
+    <t>prof26</t>
+  </si>
+  <si>
+    <t>prof27</t>
+  </si>
+  <si>
+    <t>prof28</t>
+  </si>
+  <si>
+    <t>prof31</t>
+  </si>
+  <si>
+    <t>prof32</t>
+  </si>
+  <si>
+    <t>prof33</t>
+  </si>
+  <si>
+    <t>prof34</t>
+  </si>
+  <si>
+    <t>prof35</t>
+  </si>
+  <si>
+    <t>prof36</t>
+  </si>
+  <si>
+    <t>prof37</t>
+  </si>
+  <si>
+    <t>prof38</t>
+  </si>
+  <si>
+    <t>prof41</t>
+  </si>
+  <si>
+    <t>prof42</t>
+  </si>
+  <si>
+    <t>prof43</t>
+  </si>
+  <si>
+    <t>prof44</t>
+  </si>
+  <si>
+    <t>prof45</t>
+  </si>
+  <si>
+    <t>isg12</t>
+  </si>
+  <si>
+    <t>isg13</t>
+  </si>
+  <si>
+    <t>isg14</t>
+  </si>
+  <si>
+    <t>isg15</t>
+  </si>
+  <si>
+    <t>isg16</t>
+  </si>
+  <si>
+    <t>isg17</t>
+  </si>
+  <si>
+    <t>isg18</t>
+  </si>
+  <si>
+    <t>isg21</t>
+  </si>
+  <si>
+    <t>isg22</t>
+  </si>
+  <si>
+    <t>isg23</t>
+  </si>
+  <si>
+    <t>isg24</t>
+  </si>
+  <si>
+    <t>isg25</t>
+  </si>
+  <si>
+    <t>isg26</t>
+  </si>
+  <si>
+    <t>isg27</t>
+  </si>
+  <si>
+    <t>isg28</t>
+  </si>
+  <si>
+    <t>isg31</t>
+  </si>
+  <si>
+    <t>isg32</t>
+  </si>
+  <si>
+    <t>isg33</t>
+  </si>
+  <si>
+    <t>isg34</t>
+  </si>
+  <si>
+    <t>isg35</t>
+  </si>
+  <si>
+    <t>isg36</t>
+  </si>
+  <si>
+    <t>isg37</t>
+  </si>
+  <si>
+    <t>isg38</t>
+  </si>
+  <si>
+    <t>isg41</t>
+  </si>
+  <si>
+    <t>isg42</t>
+  </si>
+  <si>
+    <t>isg43</t>
+  </si>
+  <si>
+    <t>isg44</t>
+  </si>
+  <si>
+    <t>isg45</t>
+  </si>
+  <si>
+    <t>ipv46</t>
+  </si>
+  <si>
+    <t>isg46</t>
+  </si>
+  <si>
+    <t>prof46</t>
+  </si>
+  <si>
+    <t>ipv47</t>
+  </si>
+  <si>
+    <t>isg47</t>
+  </si>
+  <si>
+    <t>prof47</t>
+  </si>
+  <si>
+    <t>ipv48</t>
+  </si>
+  <si>
+    <t>isg48</t>
+  </si>
+  <si>
+    <t>prof48</t>
+  </si>
+  <si>
+    <t>Odontograma do paciente</t>
+  </si>
+  <si>
+    <t>exameDescrição</t>
+  </si>
+  <si>
+    <t>complexidadeSUS</t>
+  </si>
+  <si>
+    <t>Agendar atendimento</t>
+  </si>
+  <si>
+    <t>turnoAgendamento</t>
+  </si>
+  <si>
+    <t>localAgendamento</t>
+  </si>
+  <si>
+    <t>disciplinaAgendamento</t>
+  </si>
+  <si>
+    <t>dataAgendamento</t>
+  </si>
+  <si>
+    <t>procedimentoAgendamento</t>
+  </si>
+  <si>
+    <t>pacienteAgendamento</t>
+  </si>
+  <si>
+    <t>statusAgendamento (Na sala de espera, não compareceu, Atendido/Liberado)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,8 +887,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +922,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,7 +1080,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -659,6 +1148,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -682,6 +1174,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -997,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5035DA7-7C4F-4E71-8F51-262E3B1D2C20}">
-  <dimension ref="B2:L46"/>
+  <dimension ref="B2:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,34 +1514,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="J2" s="31" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+      <c r="J2" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="32" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="33" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="32"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
     </row>
     <row r="4" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1082,7 +1577,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>40</v>
@@ -1114,7 +1609,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>39</v>
@@ -1138,13 +1633,13 @@
         <v>3</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="L6" s="16"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>38</v>
@@ -1154,7 +1649,7 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>54</v>
@@ -1165,17 +1660,15 @@
       <c r="J7" s="16">
         <v>4</v>
       </c>
-      <c r="K7" s="15" t="s">
-        <v>80</v>
-      </c>
+      <c r="K7" s="15"/>
       <c r="L7" s="17"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>42</v>
@@ -1193,15 +1686,17 @@
       <c r="J8" s="16">
         <v>5</v>
       </c>
-      <c r="K8" s="15"/>
+      <c r="K8" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="L8" s="17"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>43</v>
@@ -1219,12 +1714,14 @@
       <c r="J9" s="16">
         <v>6</v>
       </c>
-      <c r="K9" s="15"/>
+      <c r="K9" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="L9" s="17"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>37</v>
@@ -1248,10 +1745,10 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>45</v>
@@ -1270,10 +1767,10 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>46</v>
@@ -1290,7 +1787,7 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>36</v>
@@ -1308,7 +1805,7 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>35</v>
@@ -1316,7 +1813,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>34</v>
@@ -1324,244 +1821,843 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="H21" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="F22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>58</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="25" t="s">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="G39" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
       <c r="H39" s="27"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="28"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="28"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>200</v>
+      </c>
       <c r="G40" s="29"/>
       <c r="H40" s="30"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="31"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="G41" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="H41" s="14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="12" t="s">
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="G45" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C42" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="10" t="s">
+      <c r="H45" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="G46" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="E51" s="25" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="E60" s="25" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="E62" s="25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="D63" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="E63" s="25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="E64" s="25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="E65" s="25" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="E66" s="25" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="E67" s="25" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C68" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="E68" s="25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="E69" s="25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="25" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B39:H40"/>
+  <mergeCells count="5">
+    <mergeCell ref="G39:M40"/>
     <mergeCell ref="B2:H3"/>
     <mergeCell ref="J2:K3"/>
     <mergeCell ref="L2:L3"/>
+    <mergeCell ref="B39:E39"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new pages with javascript
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema-odonto\proof-of-concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C37E33-28D0-439B-9A54-E09D5440CFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FD35CA-BFE1-4DFC-8328-A673303B906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
@@ -856,7 +856,7 @@
     <t>pacienteAgendamento</t>
   </si>
   <si>
-    <t>statusAgendamento (Na sala de espera, não compareceu, Atendido/Liberado)</t>
+    <t>statusAgendamento</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Sugestões reunião com professores
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema-odonto\proof-of-concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FD35CA-BFE1-4DFC-8328-A673303B906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB8F853-4207-4EC3-BBEF-09F9329D3177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
   <si>
     <t>Paciente</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Disciplinas</t>
   </si>
   <si>
-    <t>STATUS</t>
-  </si>
-  <si>
     <t>código</t>
   </si>
   <si>
@@ -106,18 +103,6 @@
     <t>VARIÁVEIS</t>
   </si>
   <si>
-    <t>FAZER</t>
-  </si>
-  <si>
-    <t>ADD CNS NO PERFIL DO PACIENTE</t>
-  </si>
-  <si>
-    <t>ADD UM "ODONTOGRAMA" NO PERFIL DO PACIENTE</t>
-  </si>
-  <si>
-    <t>falta incluir no backend</t>
-  </si>
-  <si>
     <t>pacientesAtendidos</t>
   </si>
   <si>
@@ -262,12 +247,6 @@
     <t>qtdSUS (ano/semestre)</t>
   </si>
   <si>
-    <t>JS para capturar variáveis do paciente na vinculação</t>
-  </si>
-  <si>
-    <t>JS para vinculação no backend</t>
-  </si>
-  <si>
     <t>encaminhamentoOrigem</t>
   </si>
   <si>
@@ -322,9 +301,6 @@
     <t>pacienteEmail</t>
   </si>
   <si>
-    <t>pacienteFone</t>
-  </si>
-  <si>
     <t>pacienteEstCivil</t>
   </si>
   <si>
@@ -379,9 +355,6 @@
     <t>abandonoPaciente</t>
   </si>
   <si>
-    <t>página de registrar demanda / deletar uma tabela, corrigir SCRIPT APARECENDO</t>
-  </si>
-  <si>
     <t>odontograma11</t>
   </si>
   <si>
@@ -538,297 +511,6 @@
     <t>odontograma85</t>
   </si>
   <si>
-    <t>ipv11</t>
-  </si>
-  <si>
-    <t>ipv12</t>
-  </si>
-  <si>
-    <t>ipv13</t>
-  </si>
-  <si>
-    <t>ipv14</t>
-  </si>
-  <si>
-    <t>ipv15</t>
-  </si>
-  <si>
-    <t>ipv16</t>
-  </si>
-  <si>
-    <t>ipv17</t>
-  </si>
-  <si>
-    <t>ipv18</t>
-  </si>
-  <si>
-    <t>ipv21</t>
-  </si>
-  <si>
-    <t>ipv22</t>
-  </si>
-  <si>
-    <t>ipv23</t>
-  </si>
-  <si>
-    <t>ipv24</t>
-  </si>
-  <si>
-    <t>ipv25</t>
-  </si>
-  <si>
-    <t>ipv26</t>
-  </si>
-  <si>
-    <t>ipv27</t>
-  </si>
-  <si>
-    <t>ipv28</t>
-  </si>
-  <si>
-    <t>ipv31</t>
-  </si>
-  <si>
-    <t>ipv32</t>
-  </si>
-  <si>
-    <t>ipv33</t>
-  </si>
-  <si>
-    <t>ipv34</t>
-  </si>
-  <si>
-    <t>ipv35</t>
-  </si>
-  <si>
-    <t>ipv36</t>
-  </si>
-  <si>
-    <t>ipv37</t>
-  </si>
-  <si>
-    <t>ipv38</t>
-  </si>
-  <si>
-    <t>ipv41</t>
-  </si>
-  <si>
-    <t>ipv42</t>
-  </si>
-  <si>
-    <t>ipv43</t>
-  </si>
-  <si>
-    <t>ipv44</t>
-  </si>
-  <si>
-    <t>ipv45</t>
-  </si>
-  <si>
-    <t>isg11</t>
-  </si>
-  <si>
-    <t>prof11</t>
-  </si>
-  <si>
-    <t>prof12</t>
-  </si>
-  <si>
-    <t>prof13</t>
-  </si>
-  <si>
-    <t>prof14</t>
-  </si>
-  <si>
-    <t>prof15</t>
-  </si>
-  <si>
-    <t>prof16</t>
-  </si>
-  <si>
-    <t>prof17</t>
-  </si>
-  <si>
-    <t>prof18</t>
-  </si>
-  <si>
-    <t>prof21</t>
-  </si>
-  <si>
-    <t>prof22</t>
-  </si>
-  <si>
-    <t>prof23</t>
-  </si>
-  <si>
-    <t>prof24</t>
-  </si>
-  <si>
-    <t>prof25</t>
-  </si>
-  <si>
-    <t>prof26</t>
-  </si>
-  <si>
-    <t>prof27</t>
-  </si>
-  <si>
-    <t>prof28</t>
-  </si>
-  <si>
-    <t>prof31</t>
-  </si>
-  <si>
-    <t>prof32</t>
-  </si>
-  <si>
-    <t>prof33</t>
-  </si>
-  <si>
-    <t>prof34</t>
-  </si>
-  <si>
-    <t>prof35</t>
-  </si>
-  <si>
-    <t>prof36</t>
-  </si>
-  <si>
-    <t>prof37</t>
-  </si>
-  <si>
-    <t>prof38</t>
-  </si>
-  <si>
-    <t>prof41</t>
-  </si>
-  <si>
-    <t>prof42</t>
-  </si>
-  <si>
-    <t>prof43</t>
-  </si>
-  <si>
-    <t>prof44</t>
-  </si>
-  <si>
-    <t>prof45</t>
-  </si>
-  <si>
-    <t>isg12</t>
-  </si>
-  <si>
-    <t>isg13</t>
-  </si>
-  <si>
-    <t>isg14</t>
-  </si>
-  <si>
-    <t>isg15</t>
-  </si>
-  <si>
-    <t>isg16</t>
-  </si>
-  <si>
-    <t>isg17</t>
-  </si>
-  <si>
-    <t>isg18</t>
-  </si>
-  <si>
-    <t>isg21</t>
-  </si>
-  <si>
-    <t>isg22</t>
-  </si>
-  <si>
-    <t>isg23</t>
-  </si>
-  <si>
-    <t>isg24</t>
-  </si>
-  <si>
-    <t>isg25</t>
-  </si>
-  <si>
-    <t>isg26</t>
-  </si>
-  <si>
-    <t>isg27</t>
-  </si>
-  <si>
-    <t>isg28</t>
-  </si>
-  <si>
-    <t>isg31</t>
-  </si>
-  <si>
-    <t>isg32</t>
-  </si>
-  <si>
-    <t>isg33</t>
-  </si>
-  <si>
-    <t>isg34</t>
-  </si>
-  <si>
-    <t>isg35</t>
-  </si>
-  <si>
-    <t>isg36</t>
-  </si>
-  <si>
-    <t>isg37</t>
-  </si>
-  <si>
-    <t>isg38</t>
-  </si>
-  <si>
-    <t>isg41</t>
-  </si>
-  <si>
-    <t>isg42</t>
-  </si>
-  <si>
-    <t>isg43</t>
-  </si>
-  <si>
-    <t>isg44</t>
-  </si>
-  <si>
-    <t>isg45</t>
-  </si>
-  <si>
-    <t>ipv46</t>
-  </si>
-  <si>
-    <t>isg46</t>
-  </si>
-  <si>
-    <t>prof46</t>
-  </si>
-  <si>
-    <t>ipv47</t>
-  </si>
-  <si>
-    <t>isg47</t>
-  </si>
-  <si>
-    <t>prof47</t>
-  </si>
-  <si>
-    <t>ipv48</t>
-  </si>
-  <si>
-    <t>isg48</t>
-  </si>
-  <si>
-    <t>prof48</t>
-  </si>
-  <si>
-    <t>Odontograma do paciente</t>
-  </si>
-  <si>
     <t>exameDescrição</t>
   </si>
   <si>
@@ -857,6 +539,27 @@
   </si>
   <si>
     <t>statusAgendamento</t>
+  </si>
+  <si>
+    <t>justificativaDesvinculação</t>
+  </si>
+  <si>
+    <t>Agendado</t>
+  </si>
+  <si>
+    <t>noLocal</t>
+  </si>
+  <si>
+    <t>informaçõesImportantes</t>
+  </si>
+  <si>
+    <t>pacienteTel</t>
+  </si>
+  <si>
+    <t>pacienteTel2</t>
+  </si>
+  <si>
+    <t>pacienteTel3</t>
   </si>
 </sst>
 </file>
@@ -894,7 +597,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -925,12 +628,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -1080,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1122,23 +819,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1148,9 +828,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1169,14 +846,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1492,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5035DA7-7C4F-4E71-8F51-262E3B1D2C20}">
-  <dimension ref="B2:M91"/>
+  <dimension ref="B2:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,37 +1184,27 @@
     <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
-      <c r="J2" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="33"/>
-    </row>
-    <row r="4" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1557,518 +1218,447 @@
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="18">
-        <v>1</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="3" t="s">
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="21">
-        <v>2</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="16">
-        <v>3</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="L6" s="16"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="16">
-        <v>4</v>
-      </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="17"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>95</v>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="16">
-        <v>5</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" s="17"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="16">
-        <v>6</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="L9" s="17"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="16">
-        <v>7</v>
-      </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="17"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="16">
-        <v>8</v>
-      </c>
-      <c r="K11" s="15"/>
-      <c r="L11" s="17"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>99</v>
+        <v>175</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="J12" s="16">
-        <v>9</v>
-      </c>
-      <c r="K12" s="15"/>
-      <c r="L12" s="17"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>100</v>
+        <v>176</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="J13" s="16">
-        <v>10</v>
-      </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="17"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>101</v>
+        <v>177</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>269</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>275</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>274</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>268</v>
+        <v>162</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>271</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>270</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>273</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>272</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>276</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>267</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="34" t="s">
-        <v>266</v>
-      </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="G39" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="28"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" s="25" t="s">
+      <c r="B37" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="20"/>
+    </row>
+    <row r="40" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="23"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="D40" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="G40" s="29"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="31"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>201</v>
-      </c>
       <c r="G41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>19</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -2077,23 +1667,17 @@
       <c r="M41" s="1"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" s="25" t="s">
+      <c r="B42" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="D42" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>202</v>
-      </c>
       <c r="G42" s="12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2102,23 +1686,17 @@
       <c r="M42" s="1"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" s="25" t="s">
+      <c r="B43" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="D43" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>203</v>
-      </c>
       <c r="G43" s="10" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2127,23 +1705,14 @@
       <c r="M43" s="1"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="E44" s="25" t="s">
-        <v>204</v>
+      <c r="B44" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2152,23 +1721,14 @@
       <c r="M44" s="1"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="E45" s="25" t="s">
-        <v>205</v>
+      <c r="B45" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2177,20 +1737,11 @@
       <c r="M45" s="1"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="E46" s="25" t="s">
-        <v>206</v>
+      <c r="B46" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="1"/>
@@ -2200,462 +1751,239 @@
       <c r="M46" s="1"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C47" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="D47" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="25" t="s">
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C48" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="E48" s="25" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="25" t="s">
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C49" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="25" t="s">
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C50" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="E50" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="25" t="s">
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C51" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="25" t="s">
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="25" t="s">
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C53" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E53" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="25" t="s">
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C54" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="E54" s="25" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="25" t="s">
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C55" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="E55" s="25" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="25" t="s">
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C56" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="E56" s="25" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="25" t="s">
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C57" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>245</v>
-      </c>
-      <c r="E57" s="25" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="25" t="s">
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C58" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>246</v>
-      </c>
-      <c r="E58" s="25" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="25" t="s">
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C59" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>247</v>
-      </c>
-      <c r="E59" s="25" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="25" t="s">
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C60" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>248</v>
-      </c>
-      <c r="E60" s="25" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="25" t="s">
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C61" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="D61" s="25" t="s">
-        <v>249</v>
-      </c>
-      <c r="E61" s="25" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="25" t="s">
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C62" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="D62" s="25" t="s">
-        <v>250</v>
-      </c>
-      <c r="E62" s="25" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="25" t="s">
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="D63" s="25" t="s">
-        <v>251</v>
-      </c>
-      <c r="E63" s="25" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="25" t="s">
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="D64" s="25" t="s">
-        <v>252</v>
-      </c>
-      <c r="E64" s="25" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="25" t="s">
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C65" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="D65" s="25" t="s">
-        <v>253</v>
-      </c>
-      <c r="E65" s="25" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="25" t="s">
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C66" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="D66" s="25" t="s">
-        <v>254</v>
-      </c>
-      <c r="E66" s="25" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="25" t="s">
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C67" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="D67" s="25" t="s">
-        <v>255</v>
-      </c>
-      <c r="E67" s="25" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="25" t="s">
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C68" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="D68" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="E68" s="25" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="25" t="s">
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C69" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="D69" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="E69" s="25" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="25" t="s">
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C70" s="25" t="s">
-        <v>260</v>
-      </c>
-      <c r="D70" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="E70" s="25" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="25" t="s">
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C71" s="25" t="s">
-        <v>263</v>
-      </c>
-      <c r="D71" s="25" t="s">
-        <v>264</v>
-      </c>
-      <c r="E71" s="25" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="25" t="s">
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="25" t="s">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="25" t="s">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="25" t="s">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="25" t="s">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="25" t="s">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="25" t="s">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="25" t="s">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="25" t="s">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="25" t="s">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="25" t="s">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="25" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="25" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="25" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="25" t="s">
-        <v>169</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="G39:M40"/>
+  <mergeCells count="2">
     <mergeCell ref="B2:H3"/>
-    <mergeCell ref="J2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:L40"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor reviews & avaliar-atendimento-2.html
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema-odonto\proof-of-concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB8F853-4207-4EC3-BBEF-09F9329D3177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC8A6F8-A4F8-41C2-B971-C301D41D7489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Variáveis" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="183">
   <si>
     <t>Paciente</t>
   </si>
@@ -148,12 +148,6 @@
     <t>avaliarConhecimento</t>
   </si>
   <si>
-    <t>avaliarPostura</t>
-  </si>
-  <si>
-    <t>avaliarDesempenho</t>
-  </si>
-  <si>
     <t>homologarEncaminhamento</t>
   </si>
   <si>
@@ -560,6 +554,27 @@
   </si>
   <si>
     <t>pacienteTel3</t>
+  </si>
+  <si>
+    <t>avaliarComportamento</t>
+  </si>
+  <si>
+    <t>avaliarMateriais</t>
+  </si>
+  <si>
+    <t>avaliarCuidado</t>
+  </si>
+  <si>
+    <t>avaliarAdversidades</t>
+  </si>
+  <si>
+    <t>avaliarDupla</t>
+  </si>
+  <si>
+    <t>avaliarAuto</t>
+  </si>
+  <si>
+    <t>avaliarObservações</t>
   </si>
 </sst>
 </file>
@@ -828,6 +843,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -845,9 +863,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1166,7 +1181,7 @@
   <dimension ref="B2:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,24 +1200,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1233,7 +1248,7 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>35</v>
@@ -1242,10 +1257,10 @@
         <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>5</v>
@@ -1256,7 +1271,7 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>34</v>
@@ -1265,13 +1280,13 @@
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>10</v>
@@ -1279,7 +1294,7 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>33</v>
@@ -1288,13 +1303,13 @@
         <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>11</v>
@@ -1302,20 +1317,20 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>12</v>
@@ -1323,20 +1338,20 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>14</v>
@@ -1344,18 +1359,18 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>15</v>
@@ -1363,13 +1378,13 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>177</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1380,13 +1395,13 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1395,12 +1410,14 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1408,251 +1425,263 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="D17" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="F17" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="21"/>
     </row>
     <row r="40" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="23"/>
+        <v>61</v>
+      </c>
+      <c r="F40" s="22"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="24"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F41" s="24" t="s">
-        <v>170</v>
+        <v>107</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>168</v>
       </c>
       <c r="G41" s="14" t="s">
         <v>17</v>
@@ -1668,13 +1697,13 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>19</v>
@@ -1687,13 +1716,13 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>20</v>
@@ -1706,10 +1735,10 @@
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>21</v>
@@ -1722,10 +1751,10 @@
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H45" s="11" t="s">
         <v>22</v>
@@ -1738,10 +1767,10 @@
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="1"/>
@@ -1752,232 +1781,232 @@
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HTMLs agendamento e consulta de agenda
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema-odonto\proof-of-concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC8A6F8-A4F8-41C2-B971-C301D41D7489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898E363B-91D5-4A21-BD04-D244D8F8EE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Variáveis" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="184">
   <si>
     <t>Paciente</t>
   </si>
@@ -575,6 +575,9 @@
   </si>
   <si>
     <t>avaliarObservações</t>
+  </si>
+  <si>
+    <t>dataAvaliação</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1184,7 @@
   <dimension ref="B2:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,7 +1347,7 @@
         <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
@@ -1365,7 +1368,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>176</v>
+        <v>38</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1384,7 +1387,7 @@
         <v>74</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1401,7 +1404,7 @@
         <v>73</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1416,7 +1419,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>178</v>
+        <v>39</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1431,7 +1434,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
@@ -1442,7 +1445,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
@@ -1453,7 +1456,7 @@
         <v>28</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1463,8 +1466,8 @@
       <c r="C17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>182</v>
+      <c r="D17" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>76</v>
@@ -1482,6 +1485,9 @@
       </c>
       <c r="C18" s="7" t="s">
         <v>26</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
alert messages with CSS
</commit_message>
<xml_diff>
--- a/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
+++ b/Páginas em desenvolvimento ou exemplos/variáveis necessárias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFPel\Sistema-odonto\proof-of-concept\Páginas em desenvolvimento ou exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898E363B-91D5-4A21-BD04-D244D8F8EE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FB3028-0C08-4677-8A9B-A92571B704AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA4E2D1-78C1-42BF-B543-03D71FD4B3DB}"/>
   </bookViews>
@@ -283,9 +283,6 @@
     <t>pacienteNome</t>
   </si>
   <si>
-    <t>pacienteSUS</t>
-  </si>
-  <si>
     <t>pacienteRG</t>
   </si>
   <si>
@@ -578,6 +575,9 @@
   </si>
   <si>
     <t>dataAvaliação</t>
+  </si>
+  <si>
+    <t>CNS</t>
   </si>
 </sst>
 </file>
@@ -795,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -866,6 +866,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1184,7 +1187,7 @@
   <dimension ref="B2:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,8 +1253,8 @@
       <c r="M4"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
-        <v>172</v>
+      <c r="B5" s="25" t="s">
+        <v>171</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>35</v>
@@ -1306,7 +1309,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>67</v>
@@ -1320,7 +1323,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>71</v>
@@ -1341,13 +1344,13 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
@@ -1362,7 +1365,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>32</v>
@@ -1381,13 +1384,13 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>74</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1398,13 +1401,13 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1412,8 +1415,8 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>174</v>
+      <c r="B13" s="15" t="s">
+        <v>173</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>31</v>
@@ -1427,47 +1430,47 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>175</v>
+      <c r="B14" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>76</v>
@@ -1476,18 +1479,18 @@
         <v>66</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>64</v>
@@ -1496,12 +1499,12 @@
         <v>68</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>25</v>
@@ -1513,26 +1516,26 @@
         <v>69</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>62</v>
@@ -1541,45 +1544,45 @@
         <v>70</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>77</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>78</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>79</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>81</v>
@@ -1587,7 +1590,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>82</v>
@@ -1595,7 +1598,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>80</v>
@@ -1653,7 +1656,7 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1684,10 +1687,10 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G41" s="14" t="s">
         <v>17</v>
@@ -1703,13 +1706,13 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>19</v>
@@ -1722,13 +1725,13 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>20</v>
@@ -1741,10 +1744,10 @@
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>21</v>
@@ -1757,10 +1760,10 @@
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H45" s="11" t="s">
         <v>22</v>
@@ -1773,10 +1776,10 @@
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="1"/>
@@ -1787,232 +1790,232 @@
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>